<commit_message>
updated Requirements Stack Spreadsheet
</commit_message>
<xml_diff>
--- a/docs/EECS 581 - Project 3 (Requirements).xlsx
+++ b/docs/EECS 581 - Project 3 (Requirements).xlsx
@@ -472,7 +472,7 @@
     <col customWidth="1" min="5" max="5" width="16.25"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
@@ -506,7 +506,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="2">
         <v>1.1</v>
       </c>
@@ -523,7 +523,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="2">
         <v>2.0</v>
       </c>
@@ -540,7 +540,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="2">
         <v>2.1</v>
       </c>
@@ -557,7 +557,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="2">
         <v>2.2</v>
       </c>
@@ -574,7 +574,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="2">
         <v>3.0</v>
       </c>
@@ -591,7 +591,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="2">
         <v>3.1</v>
       </c>
@@ -605,7 +605,7 @@
         <v>7.0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="2">
         <v>3.2</v>
       </c>
@@ -619,7 +619,7 @@
         <v>8.0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="2">
         <v>3.3</v>
       </c>
@@ -636,7 +636,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="22.5" customHeight="1">
       <c r="A11" s="2">
         <v>4.0</v>
       </c>
@@ -653,7 +653,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="2">
         <v>4.1</v>
       </c>
@@ -667,7 +667,7 @@
         <v>11.0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="2">
         <v>4.2</v>
       </c>
@@ -681,7 +681,7 @@
         <v>12.0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="2">
         <v>5.0</v>
       </c>
@@ -695,7 +695,7 @@
         <v>13.0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="2">
         <v>5.1</v>
       </c>
@@ -709,7 +709,7 @@
         <v>14.0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="2">
         <v>5.2</v>
       </c>
@@ -723,7 +723,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="22.5" customHeight="1">
       <c r="A17" s="2">
         <v>6.0</v>
       </c>
@@ -736,8 +736,11 @@
       <c r="D17" s="3">
         <v>16.0</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="E17" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="18" ht="22.5" customHeight="1">
       <c r="A18" s="2">
         <v>6.1</v>
       </c>
@@ -750,8 +753,11 @@
       <c r="D18" s="3">
         <v>17.0</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="E18" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19" ht="22.5" customHeight="1">
       <c r="A19" s="2">
         <v>6.2</v>
       </c>
@@ -765,7 +771,7 @@
         <v>18.0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="22.5" customHeight="1">
       <c r="A20" s="2">
         <v>7.0</v>
       </c>
@@ -778,8 +784,11 @@
       <c r="D20" s="3">
         <v>19.0</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="E20" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="21" ht="22.5" customHeight="1">
       <c r="A21" s="2">
         <v>7.1</v>
       </c>
@@ -792,8 +801,11 @@
       <c r="D21" s="3">
         <v>20.0</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="E21" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="22" ht="22.5" customHeight="1">
       <c r="A22" s="2">
         <v>8.0</v>
       </c>
@@ -807,7 +819,7 @@
         <v>21.0</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="22.5" customHeight="1">
       <c r="A23" s="2">
         <v>8.1</v>
       </c>
@@ -821,7 +833,7 @@
         <v>22.0</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="22.5" customHeight="1">
       <c r="A24" s="2">
         <v>9.0</v>
       </c>
@@ -835,7 +847,7 @@
         <v>23.0</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="22.5" customHeight="1">
       <c r="A25" s="2">
         <v>9.1</v>
       </c>
@@ -849,7 +861,7 @@
         <v>24.0</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="22.5" customHeight="1">
       <c r="A26" s="2">
         <v>10.0</v>
       </c>
@@ -863,7 +875,7 @@
         <v>25.0</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="22.5" customHeight="1">
       <c r="A27" s="2">
         <v>11.0</v>
       </c>
@@ -877,7 +889,7 @@
         <v>26.0</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="22.5" customHeight="1">
       <c r="A28" s="2">
         <v>12.0</v>
       </c>
@@ -891,7 +903,7 @@
         <v>27.0</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="22.5" customHeight="1">
       <c r="A29" s="2">
         <v>13.0</v>
       </c>
@@ -905,7 +917,7 @@
         <v>28.0</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="22.5" customHeight="1">
       <c r="A30" s="2">
         <v>14.0</v>
       </c>
@@ -919,7 +931,7 @@
         <v>29.0</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="22.5" customHeight="1">
       <c r="A31" s="2">
         <v>15.0</v>
       </c>
@@ -933,7 +945,7 @@
         <v>30.0</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="22.5" customHeight="1">
       <c r="A32" s="2">
         <v>15.1</v>
       </c>
@@ -947,7 +959,7 @@
         <v>31.0</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" ht="22.5" customHeight="1">
       <c r="A33" s="2">
         <v>16.0</v>
       </c>
@@ -961,7 +973,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" ht="22.5" customHeight="1">
       <c r="A34" s="2">
         <v>17.0</v>
       </c>

</xml_diff>

<commit_message>
updated requirements spreadsheet and added sprint 4 artifacts
</commit_message>
<xml_diff>
--- a/docs/EECS 581 - Project 3 (Requirements).xlsx
+++ b/docs/EECS 581 - Project 3 (Requirements).xlsx
@@ -604,6 +604,9 @@
       <c r="D8" s="3">
         <v>7.0</v>
       </c>
+      <c r="E8" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="2">
@@ -618,6 +621,9 @@
       <c r="D9" s="3">
         <v>8.0</v>
       </c>
+      <c r="E9" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="2">
@@ -666,6 +672,9 @@
       <c r="D12" s="3">
         <v>11.0</v>
       </c>
+      <c r="E12" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="2">
@@ -694,6 +703,9 @@
       <c r="D14" s="3">
         <v>13.0</v>
       </c>
+      <c r="E14" s="2">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="2">
@@ -708,6 +720,9 @@
       <c r="D15" s="3">
         <v>14.0</v>
       </c>
+      <c r="E15" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="2">
@@ -722,6 +737,9 @@
       <c r="D16" s="3">
         <v>15.0</v>
       </c>
+      <c r="E16" s="2">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
       <c r="A17" s="2">
@@ -770,6 +788,9 @@
       <c r="D19" s="3">
         <v>18.0</v>
       </c>
+      <c r="E19" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="20" ht="22.5" customHeight="1">
       <c r="A20" s="2">
@@ -785,7 +806,7 @@
         <v>19.0</v>
       </c>
       <c r="E20" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21" ht="22.5" customHeight="1">
@@ -802,7 +823,7 @@
         <v>20.0</v>
       </c>
       <c r="E21" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="22" ht="22.5" customHeight="1">
@@ -846,6 +867,9 @@
       <c r="D24" s="3">
         <v>23.0</v>
       </c>
+      <c r="E24" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="25" ht="22.5" customHeight="1">
       <c r="A25" s="2">
@@ -887,6 +911,9 @@
       </c>
       <c r="D27" s="3">
         <v>26.0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3.0</v>
       </c>
     </row>
     <row r="28" ht="22.5" customHeight="1">

</xml_diff>